<commit_message>
Added Test Cases for User story SCA-208
</commit_message>
<xml_diff>
--- a/TestData/ServiceTestdata.xlsx
+++ b/TestData/ServiceTestdata.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\308211\IdeaProjects\ccs-scale-cat-test\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cognizantonline-my.sharepoint.com/personal/571154_cognizant_com/Documents/Desktop/SCA-223/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7030"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
   <si>
     <t>Scenario 1</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>/maps/api/place/get/json</t>
-  </si>
-  <si>
-    <t>Scenario 2</t>
   </si>
   <si>
     <t>place_id</t>
@@ -542,32 +539,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.140625" customWidth="1"/>
-    <col min="13" max="13" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="16.453125" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="16.26953125" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" customWidth="1"/>
+    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" customWidth="1"/>
+    <col min="13" max="13" width="26.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" ht="36.75" thickBot="1">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="36.5" thickBot="1">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -617,7 +614,7 @@
         <v>15</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -673,10 +670,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -721,21 +718,21 @@
         <v>18</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>27</v>
@@ -773,16 +770,16 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>27</v>
@@ -806,7 +803,7 @@
         <v>20</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>22</v>
@@ -821,7 +818,7 @@
         <v>18</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:17">

</xml_diff>